<commit_message>
working update for permissions and all other admin features
</commit_message>
<xml_diff>
--- a/codingapp/static/templates/sample_user_upload.xlsx
+++ b/codingapp/static/templates/sample_user_upload.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsrgu\Desktop\Codeloop\Codeloop\codingapp\static\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Personal\CodeloopDjango\codingapp\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8B0CAC-E66E-419E-9E49-A0B9BC8D4041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7717BB85-3CD0-40CD-BA98-9CF000471968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1747" yWindow="1747" windowWidth="14401" windowHeight="8183" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -42,38 +53,29 @@
     <t>group</t>
   </si>
   <si>
-    <t>john</t>
-  </si>
-  <si>
-    <t>John Smith</t>
-  </si>
-  <si>
-    <t>john@ex.com</t>
-  </si>
-  <si>
-    <t>secret</t>
-  </si>
-  <si>
-    <t>Group 1</t>
-  </si>
-  <si>
-    <t>jane</t>
-  </si>
-  <si>
-    <t>Jane Brown</t>
-  </si>
-  <si>
-    <t>jane@ex.com</t>
-  </si>
-  <si>
-    <t>Group 2</t>
+    <t>role</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>student_1</t>
+  </si>
+  <si>
+    <t>stu1@gmail.com</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +87,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,10 +117,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -118,8 +129,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,15 +413,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,44 +435,46 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{B2E3A1B4-5A0F-4A48-ACAC-9B76FC5085EC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>